<commit_message>
stuck on empty cell in excl
</commit_message>
<xml_diff>
--- a/TEMP.xlsx
+++ b/TEMP.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="73">
   <si>
     <t>NAME</t>
   </si>
@@ -54,9 +54,6 @@
     <t>08, Multan Nagar Daudpur , Ward No-51, Alwar</t>
   </si>
   <si>
-    <t>9694848048</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>Naghori, Salarpur, Neemrana, Alwar</t>
   </si>
   <si>
-    <t>9871643391</t>
-  </si>
-  <si>
     <t>Mohammad Faiz</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
     <t>Danpur, Intoli, Reni, Alwar</t>
   </si>
   <si>
-    <t>9414724637</t>
-  </si>
-  <si>
     <t>Rihanshi Meena</t>
   </si>
   <si>
@@ -111,9 +102,6 @@
     <t>Pinan, Reni, Alwar</t>
   </si>
   <si>
-    <t>7073079527</t>
-  </si>
-  <si>
     <t>Pranav Kumar</t>
   </si>
   <si>
@@ -126,9 +114,6 @@
     <t>Babariya, Bansur, Alwar</t>
   </si>
   <si>
-    <t>8114484593</t>
-  </si>
-  <si>
     <t>Samar Khan</t>
   </si>
   <si>
@@ -138,9 +123,6 @@
     <t>Baghor, Tijara, Alwar</t>
   </si>
   <si>
-    <t>8279281697</t>
-  </si>
-  <si>
     <t>Lakshita</t>
   </si>
   <si>
@@ -153,9 +135,6 @@
     <t>Chandichana, Dhoondhariya, Behror, Alwar</t>
   </si>
   <si>
-    <t>9610531386</t>
-  </si>
-  <si>
     <t>Inaya Khan</t>
   </si>
   <si>
@@ -168,9 +147,6 @@
     <t>Peeproli, Ward No- 6, Ramgarh, Alwar</t>
   </si>
   <si>
-    <t>8070402786</t>
-  </si>
-  <si>
     <t>Ahad Khan</t>
   </si>
   <si>
@@ -183,9 +159,6 @@
     <t>Ward No- 31, Alwar</t>
   </si>
   <si>
-    <t>7073284584</t>
-  </si>
-  <si>
     <t>YES</t>
   </si>
   <si>
@@ -201,9 +174,6 @@
     <t>31, 31 Ews Budh Vihar , Ward No- 1, Alwar, Alwar</t>
   </si>
   <si>
-    <t>9509884903</t>
-  </si>
-  <si>
     <t>Sep 27 2024  1:08PM</t>
   </si>
   <si>
@@ -231,9 +201,6 @@
     <t>Kachawa, Toda Nagar, Laxmangarh, Alwar</t>
   </si>
   <si>
-    <t>8000895683</t>
-  </si>
-  <si>
     <t>Pawan Meena</t>
   </si>
   <si>
@@ -244,9 +211,6 @@
   </si>
   <si>
     <t>Lalpura, Nayabas, Bansur, Alwar</t>
-  </si>
-  <si>
-    <t>6378374175</t>
   </si>
   <si>
     <t>Jivika Bai</t>
@@ -708,7 +672,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -749,7 +713,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -768,232 +732,232 @@
       <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>12</v>
+      <c r="F2" s="5">
+        <v>9694848048</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>18</v>
+      <c r="F3" s="8">
+        <v>9871643391</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>27</v>
+      <c r="F5" s="8">
+        <v>9414724637</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="F6" s="5">
+        <v>7073079527</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="F7" s="8">
+        <v>8114484593</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
+      </c>
+      <c r="F8" s="5">
+        <v>8279281697</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>45</v>
+        <v>38</v>
+      </c>
+      <c r="F9" s="8">
+        <v>9610531386</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
+      </c>
+      <c r="F10" s="5">
+        <v>8070402786</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>10</v>
@@ -1002,24 +966,24 @@
         <v>10</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
+      </c>
+      <c r="F12" s="5">
+        <v>7073284584</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="7" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>10</v>
@@ -1028,177 +992,177 @@
         <v>10</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>61</v>
+        <v>51</v>
+      </c>
+      <c r="F13" s="8">
+        <v>9509884903</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="7" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>71</v>
+        <v>60</v>
+      </c>
+      <c r="F15" s="8">
+        <v>8000895683</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="4" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="7" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>76</v>
+        <v>64</v>
+      </c>
+      <c r="F17" s="8">
+        <v>6378374175</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="4" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>76</v>
+        <v>64</v>
+      </c>
+      <c r="F18" s="5">
+        <v>6378374175</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="7" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>76</v>
+        <v>64</v>
+      </c>
+      <c r="F19" s="8">
+        <v>6378374175</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="4" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H20" s="6"/>
     </row>

</xml_diff>